<commit_message>
add data to create arctivle in english
</commit_message>
<xml_diff>
--- a/dataset/database-asg/cpu.xlsx
+++ b/dataset/database-asg/cpu.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B317"/>
+  <dimension ref="A1:B490"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3595,6 +3595,1736 @@
         <v>3.6667</v>
       </c>
     </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:20:05</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>25.4098</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:24:20</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>6.393399999999999</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:25:27</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>34.38985</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:26:31</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>3.50095</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:27:35</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>3.5285</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:32:32</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>3.41665</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:33:36</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>31.03676666666667</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:34:40</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>4.444766666666666</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:36:39</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>3.329533333333333</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:37:44</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>3.4806</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:38:48</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>3.461166666666666</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:39:53</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>3.26295</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:40:57</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>3.26295</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:42:00</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>3.4449</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:43:04</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:44:13</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:46:00</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:47:08</t>
+        </is>
+      </c>
+      <c r="B335" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:49:02</t>
+        </is>
+      </c>
+      <c r="B336" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:50:53</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:52:02</t>
+        </is>
+      </c>
+      <c r="B338" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:53:18</t>
+        </is>
+      </c>
+      <c r="B339" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:54:58</t>
+        </is>
+      </c>
+      <c r="B340" t="n">
+        <v>3.4497</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:56:45</t>
+        </is>
+      </c>
+      <c r="B341" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:57:58</t>
+        </is>
+      </c>
+      <c r="B342" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>06/11/2021 07:59:24</t>
+        </is>
+      </c>
+      <c r="B343" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:01:07</t>
+        </is>
+      </c>
+      <c r="B344" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:02:33</t>
+        </is>
+      </c>
+      <c r="B345" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:04:07</t>
+        </is>
+      </c>
+      <c r="B346" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:05:54</t>
+        </is>
+      </c>
+      <c r="B347" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:07:56</t>
+        </is>
+      </c>
+      <c r="B348" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:09:36</t>
+        </is>
+      </c>
+      <c r="B349" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:10:40</t>
+        </is>
+      </c>
+      <c r="B350" t="n">
+        <v>3.050800000000001</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:11:50</t>
+        </is>
+      </c>
+      <c r="B351" t="n">
+        <v>3.7705</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:13:32</t>
+        </is>
+      </c>
+      <c r="B352" t="n">
+        <v>3.4426</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:15:08</t>
+        </is>
+      </c>
+      <c r="B353" t="n">
+        <v>3.5593</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:16:36</t>
+        </is>
+      </c>
+      <c r="B354" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:17:54</t>
+        </is>
+      </c>
+      <c r="B355" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:19:16</t>
+        </is>
+      </c>
+      <c r="B356" t="n">
+        <v>3.4426</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:20:57</t>
+        </is>
+      </c>
+      <c r="B357" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:22:21</t>
+        </is>
+      </c>
+      <c r="B358" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:23:50</t>
+        </is>
+      </c>
+      <c r="B359" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:25:19</t>
+        </is>
+      </c>
+      <c r="B360" t="n">
+        <v>3.4426</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:26:55</t>
+        </is>
+      </c>
+      <c r="B361" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:31:53</t>
+        </is>
+      </c>
+      <c r="B362" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:33:23</t>
+        </is>
+      </c>
+      <c r="B363" t="n">
+        <v>26.32625</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:34:27</t>
+        </is>
+      </c>
+      <c r="B364" t="n">
+        <v>3.471300000000001</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:39:20</t>
+        </is>
+      </c>
+      <c r="B365" t="n">
+        <v>3.4463</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:41:09</t>
+        </is>
+      </c>
+      <c r="B366" t="n">
+        <v>3.417133333333334</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:42:13</t>
+        </is>
+      </c>
+      <c r="B367" t="n">
+        <v>3.878533333333333</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:43:53</t>
+        </is>
+      </c>
+      <c r="B368" t="n">
+        <v>3.3531</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:44:57</t>
+        </is>
+      </c>
+      <c r="B369" t="n">
+        <v>3.445066666666666</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:49:13</t>
+        </is>
+      </c>
+      <c r="B370" t="n">
+        <v>3.342733333333333</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:50:18</t>
+        </is>
+      </c>
+      <c r="B371" t="n">
+        <v>3.2363</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:51:23</t>
+        </is>
+      </c>
+      <c r="B372" t="n">
+        <v>20.1931</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:52:30</t>
+        </is>
+      </c>
+      <c r="B373" t="n">
+        <v>20.12083333333333</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:53:34</t>
+        </is>
+      </c>
+      <c r="B374" t="n">
+        <v>3.3878</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:54:38</t>
+        </is>
+      </c>
+      <c r="B375" t="n">
+        <v>3.4165</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:55:43</t>
+        </is>
+      </c>
+      <c r="B376" t="n">
+        <v>3.34745</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:56:50</t>
+        </is>
+      </c>
+      <c r="B377" t="n">
+        <v>3.40165</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:57:56</t>
+        </is>
+      </c>
+      <c r="B378" t="n">
+        <v>3.40165</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>06/11/2021 08:58:59</t>
+        </is>
+      </c>
+      <c r="B379" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:00:52</t>
+        </is>
+      </c>
+      <c r="B380" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:02:04</t>
+        </is>
+      </c>
+      <c r="B381" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:03:13</t>
+        </is>
+      </c>
+      <c r="B382" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:04:18</t>
+        </is>
+      </c>
+      <c r="B383" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:05:26</t>
+        </is>
+      </c>
+      <c r="B384" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:06:34</t>
+        </is>
+      </c>
+      <c r="B385" t="n">
+        <v>3.2495</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:08:25</t>
+        </is>
+      </c>
+      <c r="B386" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:09:33</t>
+        </is>
+      </c>
+      <c r="B387" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:10:40</t>
+        </is>
+      </c>
+      <c r="B388" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:11:47</t>
+        </is>
+      </c>
+      <c r="B389" t="n">
+        <v>3.4167</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:13:35</t>
+        </is>
+      </c>
+      <c r="B390" t="n">
+        <v>3.1667</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:17:56</t>
+        </is>
+      </c>
+      <c r="B391" t="n">
+        <v>3.2782</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:19:50</t>
+        </is>
+      </c>
+      <c r="B392" t="n">
+        <v>33.3098</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:20:57</t>
+        </is>
+      </c>
+      <c r="B393" t="n">
+        <v>12.2641</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:22:28</t>
+        </is>
+      </c>
+      <c r="B394" t="n">
+        <v>3.2776</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:23:33</t>
+        </is>
+      </c>
+      <c r="B395" t="n">
+        <v>3.7641</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:25:04</t>
+        </is>
+      </c>
+      <c r="B396" t="n">
+        <v>3.22405</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:26:11</t>
+        </is>
+      </c>
+      <c r="B397" t="n">
+        <v>3.30505</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:27:19</t>
+        </is>
+      </c>
+      <c r="B398" t="n">
+        <v>3.2081</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:28:24</t>
+        </is>
+      </c>
+      <c r="B399" t="n">
+        <v>3.3343</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:29:39</t>
+        </is>
+      </c>
+      <c r="B400" t="n">
+        <v>3.3343</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:31:06</t>
+        </is>
+      </c>
+      <c r="B401" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:32:47</t>
+        </is>
+      </c>
+      <c r="B402" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:34:09</t>
+        </is>
+      </c>
+      <c r="B403" t="n">
+        <v>2.7119</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:36:06</t>
+        </is>
+      </c>
+      <c r="B404" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:38:05</t>
+        </is>
+      </c>
+      <c r="B405" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:40:30</t>
+        </is>
+      </c>
+      <c r="B406" t="n">
+        <v>3.222700000000001</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:42:22</t>
+        </is>
+      </c>
+      <c r="B407" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:44:12</t>
+        </is>
+      </c>
+      <c r="B408" t="n">
+        <v>3.1148</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:46:21</t>
+        </is>
+      </c>
+      <c r="B409" t="n">
+        <v>3.3315</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:48:21</t>
+        </is>
+      </c>
+      <c r="B410" t="n">
+        <v>3.2523</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:50:13</t>
+        </is>
+      </c>
+      <c r="B411" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:52:12</t>
+        </is>
+      </c>
+      <c r="B412" t="n">
+        <v>3.3898</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:53:56</t>
+        </is>
+      </c>
+      <c r="B413" t="n">
+        <v>3.1667</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>06/11/2021 09:58:44</t>
+        </is>
+      </c>
+      <c r="B414" t="n">
+        <v>3.2495</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:00:14</t>
+        </is>
+      </c>
+      <c r="B415" t="n">
+        <v>44.80370000000001</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:01:19</t>
+        </is>
+      </c>
+      <c r="B416" t="n">
+        <v>10.8873</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:05:31</t>
+        </is>
+      </c>
+      <c r="B417" t="n">
+        <v>3.4894</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:06:59</t>
+        </is>
+      </c>
+      <c r="B418" t="n">
+        <v>18.40743333333333</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:08:06</t>
+        </is>
+      </c>
+      <c r="B419" t="n">
+        <v>3.371599999999999</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:09:50</t>
+        </is>
+      </c>
+      <c r="B420" t="n">
+        <v>3.305066666666667</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:11:40</t>
+        </is>
+      </c>
+      <c r="B421" t="n">
+        <v>11.00033333333333</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:13:19</t>
+        </is>
+      </c>
+      <c r="B422" t="n">
+        <v>3.406066666666666</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:14:43</t>
+        </is>
+      </c>
+      <c r="B423" t="n">
+        <v>3.352</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:16:08</t>
+        </is>
+      </c>
+      <c r="B424" t="n">
+        <v>3.3889</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:17:45</t>
+        </is>
+      </c>
+      <c r="B425" t="n">
+        <v>3.389666666666667</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:19:10</t>
+        </is>
+      </c>
+      <c r="B426" t="n">
+        <v>3.426533333333333</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:20:33</t>
+        </is>
+      </c>
+      <c r="B427" t="n">
+        <v>3.2969</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:21:38</t>
+        </is>
+      </c>
+      <c r="B428" t="n">
+        <v>3.4937</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:23:15</t>
+        </is>
+      </c>
+      <c r="B429" t="n">
+        <v>6.793566666666666</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:24:51</t>
+        </is>
+      </c>
+      <c r="B430" t="n">
+        <v>6.834899999999999</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:26:28</t>
+        </is>
+      </c>
+      <c r="B431" t="n">
+        <v>3.351066666666667</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:27:52</t>
+        </is>
+      </c>
+      <c r="B432" t="n">
+        <v>3.285833333333333</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:28:59</t>
+        </is>
+      </c>
+      <c r="B433" t="n">
+        <v>3.307</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:30:03</t>
+        </is>
+      </c>
+      <c r="B434" t="n">
+        <v>3.4068</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:31:37</t>
+        </is>
+      </c>
+      <c r="B435" t="n">
+        <v>3.4088</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:33:07</t>
+        </is>
+      </c>
+      <c r="B436" t="n">
+        <v>3.352466666666666</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:34:12</t>
+        </is>
+      </c>
+      <c r="B437" t="n">
+        <v>3.373233333333333</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:35:46</t>
+        </is>
+      </c>
+      <c r="B438" t="n">
+        <v>3.370966666666666</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:36:52</t>
+        </is>
+      </c>
+      <c r="B439" t="n">
+        <v>3.324533333333333</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:37:58</t>
+        </is>
+      </c>
+      <c r="B440" t="n">
+        <v>3.4264</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:39:32</t>
+        </is>
+      </c>
+      <c r="B441" t="n">
+        <v>3.278233333333334</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:40:39</t>
+        </is>
+      </c>
+      <c r="B442" t="n">
+        <v>3.186233333333333</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:41:44</t>
+        </is>
+      </c>
+      <c r="B443" t="n">
+        <v>3.279</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:42:49</t>
+        </is>
+      </c>
+      <c r="B444" t="n">
+        <v>3.33565</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:43:55</t>
+        </is>
+      </c>
+      <c r="B445" t="n">
+        <v>3.33375</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:45:00</t>
+        </is>
+      </c>
+      <c r="B446" t="n">
+        <v>3.278</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:46:04</t>
+        </is>
+      </c>
+      <c r="B447" t="n">
+        <v>3.2787</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:47:52</t>
+        </is>
+      </c>
+      <c r="B448" t="n">
+        <v>3.1935</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:49:24</t>
+        </is>
+      </c>
+      <c r="B449" t="n">
+        <v>3.1667</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:50:57</t>
+        </is>
+      </c>
+      <c r="B450" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:52:33</t>
+        </is>
+      </c>
+      <c r="B451" t="n">
+        <v>3.1667</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:54:11</t>
+        </is>
+      </c>
+      <c r="B452" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:55:49</t>
+        </is>
+      </c>
+      <c r="B453" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:57:22</t>
+        </is>
+      </c>
+      <c r="B454" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>06/11/2021 10:59:07</t>
+        </is>
+      </c>
+      <c r="B455" t="n">
+        <v>3.1667</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:00:46</t>
+        </is>
+      </c>
+      <c r="B456" t="n">
+        <v>3.3333</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:02:24</t>
+        </is>
+      </c>
+      <c r="B457" t="n">
+        <v>3.1393</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:04:12</t>
+        </is>
+      </c>
+      <c r="B458" t="n">
+        <v>3.0268</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:06:02</t>
+        </is>
+      </c>
+      <c r="B459" t="n">
+        <v>3.1667</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:10:36</t>
+        </is>
+      </c>
+      <c r="B460" t="n">
+        <v>3.1667</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:11:44</t>
+        </is>
+      </c>
+      <c r="B461" t="n">
+        <v>28.41595</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:12:49</t>
+        </is>
+      </c>
+      <c r="B462" t="n">
+        <v>7.538650000000001</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:17:05</t>
+        </is>
+      </c>
+      <c r="B463" t="n">
+        <v>3.559300000000001</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:18:55</t>
+        </is>
+      </c>
+      <c r="B464" t="n">
+        <v>13.8094</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:20:01</t>
+        </is>
+      </c>
+      <c r="B465" t="n">
+        <v>3.317566666666667</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:21:48</t>
+        </is>
+      </c>
+      <c r="B466" t="n">
+        <v>3.4338</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:23:26</t>
+        </is>
+      </c>
+      <c r="B467" t="n">
+        <v>3.426066666666666</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:25:16</t>
+        </is>
+      </c>
+      <c r="B468" t="n">
+        <v>3.294633333333334</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:26:21</t>
+        </is>
+      </c>
+      <c r="B469" t="n">
+        <v>3.4227</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:28:01</t>
+        </is>
+      </c>
+      <c r="B470" t="n">
+        <v>3.0894</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:29:06</t>
+        </is>
+      </c>
+      <c r="B471" t="n">
+        <v>3.5525</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:31:01</t>
+        </is>
+      </c>
+      <c r="B472" t="n">
+        <v>3.5562</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:36:00</t>
+        </is>
+      </c>
+      <c r="B473" t="n">
+        <v>3.465166666666667</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:37:40</t>
+        </is>
+      </c>
+      <c r="B474" t="n">
+        <v>11.8981</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:38:46</t>
+        </is>
+      </c>
+      <c r="B475" t="n">
+        <v>3.5631</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:39:58</t>
+        </is>
+      </c>
+      <c r="B476" t="n">
+        <v>3.64665</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:41:52</t>
+        </is>
+      </c>
+      <c r="B477" t="n">
+        <v>3.4843</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:43:47</t>
+        </is>
+      </c>
+      <c r="B478" t="n">
+        <v>3.4463</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:45:38</t>
+        </is>
+      </c>
+      <c r="B479" t="n">
+        <v>3.446075</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:47:19</t>
+        </is>
+      </c>
+      <c r="B480" t="n">
+        <v>3.484975</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:48:28</t>
+        </is>
+      </c>
+      <c r="B481" t="n">
+        <v>3.507425</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:50:19</t>
+        </is>
+      </c>
+      <c r="B482" t="n">
+        <v>3.478725</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:52:06</t>
+        </is>
+      </c>
+      <c r="B483" t="n">
+        <v>3.52965</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:54:04</t>
+        </is>
+      </c>
+      <c r="B484" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:55:13</t>
+        </is>
+      </c>
+      <c r="B485" t="n">
+        <v>3.458325</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:56:28</t>
+        </is>
+      </c>
+      <c r="B486" t="n">
+        <v>3.472575</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:58:24</t>
+        </is>
+      </c>
+      <c r="B487" t="n">
+        <v>3.430675</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>06/11/2021 11:59:32</t>
+        </is>
+      </c>
+      <c r="B488" t="n">
+        <v>3.457875</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>06/11/2021 12:00:39</t>
+        </is>
+      </c>
+      <c r="B489" t="n">
+        <v>3.423725</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>06/11/2021 12:01:50</t>
+        </is>
+      </c>
+      <c r="B490" t="n">
+        <v>3.556366666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>